<commit_message>
Bento object repository revisited
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_FileAssoc-diagnosis.xlsx
+++ b/InputFiles/TC01_Canine_Filter_FileAssoc-diagnosis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\yes breed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F659CD03-BCAB-4B41-9AA2-41937CE43EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDC8E1E-7276-4FBA-A40D-CB9E1F9BA4A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -57,25 +57,6 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
- MATCH (samp:sample)--&gt;(c) 
- WHERE labels(parent)[0] IN ["diagnosis"]  
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`,
-        coalesce(f.file_type, '') AS `File Type`,
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
     <t>MATCH (s:study)
   WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies
   MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies
@@ -143,6 +124,23 @@
         coalesce(demo.weight, '') AS `Weight (kg)`,
         coalesce(diag.best_response, '') AS `Response to Treatment`,
         coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+ MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+ MATCH (samp:sample)--&gt;(c) 
+ WHERE labels(parent)[0] IN ["diagnosis"]  
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN coalesce(f.file_name, '') AS `File Name`, 
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
 </sst>
 </file>
@@ -514,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,16 +547,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="290" x14ac:dyDescent="0.35">
@@ -566,16 +564,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="261" x14ac:dyDescent="0.35">
@@ -583,16 +581,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Diagnosis, FileAssociation, FileFormat, FileType, NeuteredStatus, PrimeDiseaseSite
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_FileAssoc-diagnosis.xlsx
+++ b/InputFiles/TC01_Canine_Filter_FileAssoc-diagnosis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDC8E1E-7276-4FBA-A40D-CB9E1F9BA4A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA428AA7-281B-49C8-BB6C-2339BA8AE8F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -104,6 +104,23 @@
   <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+ MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+ MATCH (samp:sample)--&gt;(c) 
+ WHERE labels(parent)[0] IN ["diagnosis"]  
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN coalesce(f.file_name, '') AS `File Name`, 
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
  WHERE labels(parent)[0] IN ["diagnosis"] 
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
 MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
@@ -122,25 +139,7 @@
         coalesce(demo.sex, '') AS Sex ,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
- MATCH (samp:sample)--&gt;(c) 
- WHERE labels(parent)[0] IN ["diagnosis"]  
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
   </si>
 </sst>
 </file>
@@ -512,20 +511,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.6328125" customWidth="1"/>
-    <col min="3" max="3" width="75.81640625" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.77734375" customWidth="1"/>
+    <col min="4" max="4" width="70.21875" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -542,12 +541,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -559,7 +558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="288" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -576,12 +575,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>

</xml_diff>